<commit_message>
Added codes to insert to school table and organized the things
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11340" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
   <si>
     <t>Attribute</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>Eye Remark for Patient</t>
+  </si>
+  <si>
+    <t>Foreign/School ID</t>
   </si>
 </sst>
 </file>
@@ -940,7 +943,7 @@
   <dimension ref="A2:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1052,7 @@
         <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>